<commit_message>
Tidied up schematic, changed footprints
</commit_message>
<xml_diff>
--- a/BOM_Generator.xlsx
+++ b/BOM_Generator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\btlf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\btlf\OneDrive\Documents\GitHub\Eka-PGr-SignalGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE9E049-1EE9-41B9-9FFB-3F3A6107BADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCF3A94-4964-4F3B-ACAA-F92F95634B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{989FA2D6-1581-4470-8D51-A9F5C31DB016}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{989FA2D6-1581-4470-8D51-A9F5C31DB016}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +314,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -343,8 +352,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -358,12 +368,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -698,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F03D75F-8B85-44C4-AA49-74880ED511BF}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +791,7 @@
         <f>D3*G$1</f>
         <v>2</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <f t="shared" ref="H3:H7" si="0">E3*G3</f>
         <v>8.6639999999999997</v>
       </c>
@@ -812,7 +825,7 @@
         <f>D4*G$1</f>
         <v>2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>6.1520000000000001</v>
       </c>
@@ -846,7 +859,7 @@
         <f t="shared" ref="G5:G29" si="1">D5*G$1</f>
         <v>2</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>2.7280000000000002</v>
       </c>
@@ -880,7 +893,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>2.226</v>
       </c>
@@ -929,7 +942,7 @@
       <c r="C8" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <v>4</v>
       </c>
       <c r="E8">
@@ -942,7 +955,7 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8">
         <f>E8*G8</f>
         <v>6.2816000000000001</v>
       </c>
@@ -961,7 +974,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9">
         <f t="shared" ref="H9:H29" si="2">E9*G9</f>
         <v>0</v>
       </c>
@@ -989,7 +1002,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10">
         <f t="shared" si="2"/>
         <v>8.2319999999999993</v>
       </c>
@@ -1023,7 +1036,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11">
         <f t="shared" si="2"/>
         <v>1.458</v>
       </c>
@@ -1057,7 +1070,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12">
         <f t="shared" si="2"/>
         <v>1.278</v>
       </c>
@@ -1091,11 +1104,11 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13">
         <f t="shared" si="2"/>
         <v>1.5596000000000001</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>78</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -1110,7 +1123,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1123,7 +1136,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1136,7 +1149,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1164,7 +1177,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17">
         <f t="shared" si="2"/>
         <v>14.74</v>
       </c>
@@ -1211,7 +1224,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1224,7 +1237,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1237,7 +1250,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1250,7 +1263,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1263,7 +1276,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1276,7 +1289,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1289,7 +1302,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1302,7 +1315,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1315,7 +1328,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1328,7 +1341,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1341,13 +1354,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J13" r:id="rId1" xr:uid="{12E41B88-C7F8-4537-9A81-170817A636BD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>